<commit_message>
Nuovo aggiornamento Check List
Aggiornato file check-list.xlsx come da Vs richiesta via mail
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GARASOFTWAREXX/Gara_Software/AnaSanPlus/V1/report-checklist.xlsx
+++ b/GATEWAY/A1#111GARASOFTWAREXX/Gara_Software/AnaSanPlus/V1/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\AnaSan\FSE\FSE 2\Accreditamento\V1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4271250-C227-4B04-913F-8515F979F68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946CEB0B-1AF4-4522-A19A-2C1065BB4FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3576,13 +3576,13 @@
     <t>Viene effettuata la segnalazione dell'errore all'assistenza attraverso la memorizzazione in un file di Log. Il documento viene messo in una coda che si occupa di eseguire la retry fino a 5 tentativi. Se il documento resta nella coda verrà poi gestito in backoffice da un operatore del supporto tecnico.</t>
   </si>
   <si>
-    <t>Errore di sintassi. Il campo "Condizioni del paziente alla dimissione e diagnosi di dimissione" è obbligatorio</t>
-  </si>
-  <si>
-    <t>Errore di sintassi. E' obbligatorio compilare la sezione 'Referto'.</t>
-  </si>
-  <si>
-    <t>Errore di sintassi. Il campo "Modalità di Trasporto" è obbligatorio</t>
+    <t>Errore Semantico. Il campo "Condizioni del paziente alla dimissione e diagnosi di dimissione" è obbligatorio</t>
+  </si>
+  <si>
+    <t>Errore Semantico. E' obbligatorio compilare la sezione 'Referto'.</t>
+  </si>
+  <si>
+    <t>Errore Semantico. Il campo "Modalità di Trasporto" è obbligatorio</t>
   </si>
 </sst>
 </file>
@@ -6614,10 +6614,10 @@
   <dimension ref="A1:T755"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="H59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="N59" sqref="N59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>